<commit_message>
support change root path to support docker
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Guild.xlsx
+++ b/_Out/NFDataCfg/Excel/Guild.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="10343" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="10343" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -23,15 +23,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Skill" type="4" refreshedVersion="2" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="Skill" type="4" refreshedVersion="2" background="1" saveData="1">
     <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Skill.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="86">
   <si>
     <t>Id</t>
   </si>
@@ -225,9 +225,6 @@
     <t>工会副本所在的曾</t>
   </si>
   <si>
-    <t>GuildBoss</t>
-  </si>
-  <si>
     <t>Row</t>
   </si>
   <si>
@@ -249,9 +246,6 @@
     <t>VIP</t>
   </si>
   <si>
-    <t>Offline</t>
-  </si>
-  <si>
     <t>Power</t>
   </si>
   <si>
@@ -285,18 +279,6 @@
     <t>GuildAppyList</t>
   </si>
   <si>
-    <t>GuildEvent</t>
-  </si>
-  <si>
-    <t>EventID</t>
-  </si>
-  <si>
-    <t>EventTime</t>
-  </si>
-  <si>
-    <t>Context</t>
-  </si>
-  <si>
     <t>GuildHouse</t>
   </si>
   <si>
@@ -304,12 +286,15 @@
   </si>
   <si>
     <t>Force</t>
+  </si>
+  <si>
+    <t>LastTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -484,7 +469,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -493,9 +478,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -543,7 +525,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2">
-    <tableStyle name="MySqlDefault" count="2">
+    <tableStyle name="MySqlDefault" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -816,7 +798,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -841,91 +823,91 @@
     <col min="16" max="16" width="16.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="4" customFormat="1">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:27" s="3" customFormat="1">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="V1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:27" s="2" customFormat="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1008,7 +990,7 @@
       </c>
     </row>
     <row r="3" spans="1:27" s="2" customFormat="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="2">
@@ -1091,7 +1073,7 @@
       </c>
     </row>
     <row r="4" spans="1:27" s="2" customFormat="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="2">
@@ -1174,7 +1156,7 @@
       </c>
     </row>
     <row r="5" spans="1:27" s="2" customFormat="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="2">
@@ -1257,7 +1239,7 @@
       </c>
     </row>
     <row r="6" spans="1:27" s="2" customFormat="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="2">
@@ -1339,342 +1321,342 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="5" customFormat="1" ht="13.5">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:27" s="4" customFormat="1" ht="13.5">
+      <c r="A7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
-        <v>0</v>
-      </c>
-      <c r="K7" s="5">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5">
-        <v>0</v>
-      </c>
-      <c r="M7" s="5">
-        <v>0</v>
-      </c>
-      <c r="N7" s="5">
-        <v>0</v>
-      </c>
-      <c r="O7" s="5">
-        <v>0</v>
-      </c>
-      <c r="P7" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>0</v>
-      </c>
-      <c r="R7" s="5">
-        <v>0</v>
-      </c>
-      <c r="S7" s="5">
-        <v>0</v>
-      </c>
-      <c r="T7" s="5">
-        <v>0</v>
-      </c>
-      <c r="U7" s="5">
-        <v>0</v>
-      </c>
-      <c r="V7" s="5">
-        <v>0</v>
-      </c>
-      <c r="W7" s="5">
-        <v>0</v>
-      </c>
-      <c r="X7" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" s="5" customFormat="1" ht="18" customHeight="1">
-      <c r="A8" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" s="5">
-        <v>0</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0</v>
-      </c>
-      <c r="K8" s="5">
-        <v>0</v>
-      </c>
-      <c r="L8" s="5">
-        <v>0</v>
-      </c>
-      <c r="M8" s="5">
-        <v>0</v>
-      </c>
-      <c r="N8" s="5">
-        <v>0</v>
-      </c>
-      <c r="O8" s="5">
-        <v>0</v>
-      </c>
-      <c r="P8" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="5">
-        <v>0</v>
-      </c>
-      <c r="R8" s="5">
-        <v>0</v>
-      </c>
-      <c r="S8" s="5">
-        <v>0</v>
-      </c>
-      <c r="T8" s="5">
-        <v>0</v>
-      </c>
-      <c r="U8" s="5">
-        <v>0</v>
-      </c>
-      <c r="V8" s="5">
-        <v>0</v>
-      </c>
-      <c r="W8" s="5">
-        <v>0</v>
-      </c>
-      <c r="X8" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" s="5" customFormat="1" ht="18" customHeight="1">
-      <c r="A9" s="9" t="s">
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>0</v>
+      </c>
+      <c r="R7" s="4">
+        <v>0</v>
+      </c>
+      <c r="S7" s="4">
+        <v>0</v>
+      </c>
+      <c r="T7" s="4">
+        <v>0</v>
+      </c>
+      <c r="U7" s="4">
+        <v>0</v>
+      </c>
+      <c r="V7" s="4">
+        <v>0</v>
+      </c>
+      <c r="W7" s="4">
+        <v>0</v>
+      </c>
+      <c r="X7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" s="4" customFormat="1" ht="18" customHeight="1">
+      <c r="A8" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>0</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0</v>
+      </c>
+      <c r="S8" s="4">
+        <v>0</v>
+      </c>
+      <c r="T8" s="4">
+        <v>0</v>
+      </c>
+      <c r="U8" s="4">
+        <v>0</v>
+      </c>
+      <c r="V8" s="4">
+        <v>0</v>
+      </c>
+      <c r="W8" s="4">
+        <v>0</v>
+      </c>
+      <c r="X8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="4" customFormat="1" ht="18" customHeight="1">
+      <c r="A9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="5">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5">
-        <v>0</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0</v>
-      </c>
-      <c r="K9" s="5">
-        <v>0</v>
-      </c>
-      <c r="L9" s="5">
-        <v>0</v>
-      </c>
-      <c r="M9" s="5">
-        <v>0</v>
-      </c>
-      <c r="N9" s="5">
-        <v>0</v>
-      </c>
-      <c r="O9" s="5">
-        <v>0</v>
-      </c>
-      <c r="P9" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="5">
-        <v>0</v>
-      </c>
-      <c r="R9" s="5">
-        <v>0</v>
-      </c>
-      <c r="S9" s="5">
-        <v>0</v>
-      </c>
-      <c r="T9" s="5">
-        <v>0</v>
-      </c>
-      <c r="U9" s="5">
-        <v>0</v>
-      </c>
-      <c r="V9" s="5">
-        <v>0</v>
-      </c>
-      <c r="W9" s="5">
-        <v>0</v>
-      </c>
-      <c r="X9" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" s="6" customFormat="1">
-      <c r="A10" s="10" t="s">
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0</v>
+      </c>
+      <c r="S9" s="4">
+        <v>0</v>
+      </c>
+      <c r="T9" s="4">
+        <v>0</v>
+      </c>
+      <c r="U9" s="4">
+        <v>0</v>
+      </c>
+      <c r="V9" s="4">
+        <v>0</v>
+      </c>
+      <c r="W9" s="4">
+        <v>0</v>
+      </c>
+      <c r="X9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" s="5" customFormat="1">
+      <c r="A10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="M10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="N10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="6" t="s">
+      <c r="O10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="P10" s="6" t="s">
+      <c r="P10" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="Q10" s="6" t="s">
+      <c r="Q10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="R10" s="6" t="s">
+      <c r="R10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="S10" s="6" t="s">
+      <c r="S10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="T10" s="6" t="s">
+      <c r="T10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="U10" s="6" t="s">
+      <c r="U10" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="V10" s="6" t="s">
+      <c r="V10" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="W10" s="6" t="s">
+      <c r="W10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="X10" s="6" t="s">
+      <c r="X10" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="Y10" s="6" t="s">
+      <c r="Y10" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="Z10" s="6" t="s">
+      <c r="Z10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AA10" s="6" t="s">
+      <c r="AA10" s="5" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:AA9">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:AA9" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1684,51 +1666,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N66"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="8.73046875" customWidth="1"/>
+    <col min="13" max="13" width="11.06640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:15" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1">
+      <c r="A2" s="2" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="B2" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1">
+    <row r="3" spans="1:15" s="2" customFormat="1">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="2" customFormat="1">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="2" customFormat="1">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
@@ -1736,7 +1720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1">
+    <row r="6" spans="1:15" s="2" customFormat="1">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -1744,7 +1728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1">
+    <row r="7" spans="1:15" s="2" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
@@ -1752,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1">
+    <row r="8" spans="1:15" s="2" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -1760,33 +1744,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1">
+    <row r="9" spans="1:15" s="2" customFormat="1">
       <c r="A9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="H9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1">
+      <c r="J9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="2" customFormat="1">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
@@ -1811,40 +1816,61 @@
       <c r="H10" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="2" customFormat="1">
+      <c r="I10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="2" customFormat="1">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="1" customFormat="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="1" customFormat="1">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="2" customFormat="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="2" customFormat="1">
       <c r="A13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1">
+    <row r="14" spans="1:15" s="2" customFormat="1">
       <c r="A14" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="2" customFormat="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="2" customFormat="1">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -1852,7 +1878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="2" customFormat="1">
+    <row r="16" spans="1:15" s="2" customFormat="1">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -1860,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="2" customFormat="1">
+    <row r="17" spans="1:4" s="2" customFormat="1">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1868,7 +1894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="2" customFormat="1">
+    <row r="18" spans="1:4" s="2" customFormat="1">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1876,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="2" customFormat="1">
+    <row r="19" spans="1:4" s="2" customFormat="1">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1884,51 +1910,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="2" customFormat="1">
+    <row r="20" spans="1:4" s="2" customFormat="1">
       <c r="A20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" s="2" customFormat="1">
+    </row>
+    <row r="21" spans="1:4" s="2" customFormat="1">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
@@ -1941,78 +1937,48 @@
       <c r="D21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" s="2" customFormat="1">
+    </row>
+    <row r="22" spans="1:4" s="2" customFormat="1">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="1" customFormat="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="1" customFormat="1">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" s="2" customFormat="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="2" customFormat="1">
       <c r="A24" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="2" customFormat="1">
+    <row r="25" spans="1:4" s="2" customFormat="1">
       <c r="A25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" s="2" customFormat="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="2" customFormat="1">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" s="2" customFormat="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="2" customFormat="1">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -2020,7 +1986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="2" customFormat="1">
+    <row r="28" spans="1:4" s="2" customFormat="1">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -2028,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="2" customFormat="1">
+    <row r="29" spans="1:4" s="2" customFormat="1">
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
@@ -2036,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="2" customFormat="1">
+    <row r="30" spans="1:4" s="2" customFormat="1">
       <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
@@ -2044,30 +2010,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="2" customFormat="1">
+    <row r="31" spans="1:4" s="2" customFormat="1">
       <c r="A31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" s="2" customFormat="1">
+    </row>
+    <row r="32" spans="1:4" s="2" customFormat="1">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
@@ -2077,52 +2031,40 @@
       <c r="C32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" s="2" customFormat="1">
+    </row>
+    <row r="33" spans="1:2" s="2" customFormat="1">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" s="1" customFormat="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="1" customFormat="1">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" s="2" customFormat="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="2" customFormat="1">
       <c r="A35" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="2" customFormat="1">
+    <row r="36" spans="1:2" s="2" customFormat="1">
       <c r="A36" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B36" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="2" customFormat="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="2" customFormat="1">
       <c r="A37" s="2" t="s">
         <v>31</v>
       </c>
@@ -2130,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="2" customFormat="1">
+    <row r="38" spans="1:2" s="2" customFormat="1">
       <c r="A38" s="2" t="s">
         <v>32</v>
       </c>
@@ -2138,7 +2080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="2" customFormat="1">
+    <row r="39" spans="1:2" s="2" customFormat="1">
       <c r="A39" s="2" t="s">
         <v>33</v>
       </c>
@@ -2146,7 +2088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="2" customFormat="1">
+    <row r="40" spans="1:2" s="2" customFormat="1">
       <c r="A40" s="2" t="s">
         <v>34</v>
       </c>
@@ -2154,7 +2096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="2" customFormat="1">
+    <row r="41" spans="1:2" s="2" customFormat="1">
       <c r="A41" s="2" t="s">
         <v>36</v>
       </c>
@@ -2162,342 +2104,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="2" customFormat="1">
+    <row r="42" spans="1:2" s="2" customFormat="1">
       <c r="A42" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" s="2" customFormat="1">
+    </row>
+    <row r="43" spans="1:2" s="2" customFormat="1">
       <c r="A43" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" s="2" customFormat="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="2" customFormat="1">
       <c r="A44" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" s="1" customFormat="1">
-      <c r="A45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" s="2" customFormat="1">
-      <c r="A46" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B46" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" s="2" customFormat="1">
-      <c r="A47" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B47" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" s="2" customFormat="1">
-      <c r="A48" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B48" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" s="2" customFormat="1">
-      <c r="A49" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B49" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" s="2" customFormat="1">
-      <c r="A50" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B50" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="2" customFormat="1">
-      <c r="A51" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B51" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" s="2" customFormat="1">
-      <c r="A52" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B52" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" s="2" customFormat="1">
-      <c r="A53" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" s="2" customFormat="1">
-      <c r="A54" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" s="2" customFormat="1">
-      <c r="A55" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" s="1" customFormat="1">
-      <c r="A56" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" s="2" customFormat="1">
-      <c r="A57" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B57" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" s="2" customFormat="1">
-      <c r="A58" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B58" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" s="2" customFormat="1">
-      <c r="A59" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B59" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" s="2" customFormat="1">
-      <c r="A60" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B60" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" s="2" customFormat="1">
-      <c r="A61" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B61" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" s="2" customFormat="1">
-      <c r="A62" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B62" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" s="2" customFormat="1">
-      <c r="A63" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B63" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" s="2" customFormat="1">
-      <c r="A64" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" s="2" customFormat="1">
-      <c r="A65" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" s="2" customFormat="1">
-      <c r="A66" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>74</v>
-      </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C8 C11:C19 C22:C30 C33:C41 C44:C66 A13:B14 A24:B25 A35:B36 A46:B47 A57:B58 A2:B3">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C19 A2:B3 A13:B14 A24:B25 A35:B36 C1:C8 B42:B44 C22:C41" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E42 A9:A10 A20:A21 A31:A32 A64:A65 L1:L19 L22:L66 A42:D43 F42:H43 A53:B54">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A9:A10 A20:A21 A42:A43 A31:B32 L1:L8 L11:L44 G31:G32 G42:G44" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"int,string,float,object"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="I42 B9:B10 B20:B21 B31:B32 M1:M19 M22:M66"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B8 B18:B19 B29:B30 B40:B41 B51:B52 B62:B63 D22:G30 D33:G41 A15:B17 A26:B28 A37:B39 A48:B50 A59:B61 A4:B6 D1:G8 D11:G19 D44:G66">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B9:B10 B20:B21 M1:M8 M11:M44 H31:H32 H42:H44" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B8 B18:B19 B29:B30 B40:B41 D11:G19 A4:B6 A15:B17 A26:B28 A37:B39 D1:G8 D22:G30 D33:G41" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
recording the war data
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Guild.xlsx
+++ b/_Out/NFDataCfg/Excel/Guild.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="86">
   <si>
     <t>Id</t>
   </si>
@@ -319,7 +319,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,6 +338,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -469,7 +475,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -502,6 +508,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1667,10 +1676,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="A11" sqref="A11:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1738,7 +1747,7 @@
     </row>
     <row r="8" spans="1:15" s="2" customFormat="1">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
@@ -1746,149 +1755,149 @@
     </row>
     <row r="9" spans="1:15" s="2" customFormat="1">
       <c r="A9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="2" customFormat="1">
       <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="11" customFormat="1">
+      <c r="A11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="11" customFormat="1">
+      <c r="A12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" s="2" t="s">
+      <c r="C12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" s="2" customFormat="1">
-      <c r="A11" s="2" t="s">
+      <c r="O12" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="11" customFormat="1">
+      <c r="A13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B13" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="1" customFormat="1">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="14" spans="1:15" s="1" customFormat="1">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="2" customFormat="1">
-      <c r="A13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="2" customFormat="1">
-      <c r="A14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="2">
-        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="2" customFormat="1">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="B15" s="2">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="2" customFormat="1">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="B16" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="2" customFormat="1">
       <c r="A17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
@@ -1896,115 +1905,117 @@
     </row>
     <row r="18" spans="1:4" s="2" customFormat="1">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="2" customFormat="1">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="2" customFormat="1">
       <c r="A20" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>70</v>
+        <v>34</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="2" customFormat="1">
       <c r="A21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="2" customFormat="1">
       <c r="A22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="2" customFormat="1">
+      <c r="A23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="2" customFormat="1">
+      <c r="A24" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="2" customFormat="1">
+      <c r="A25" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="2" customFormat="1">
+      <c r="A26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B26" s="11" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" s="1" customFormat="1">
-      <c r="A23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:4" s="1" customFormat="1">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="2" customFormat="1">
-      <c r="A24" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="2" customFormat="1">
-      <c r="A25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="2" customFormat="1">
-      <c r="A26" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="2" customFormat="1">
-      <c r="A27" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="2" customFormat="1">
       <c r="A28" s="2" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B28" s="2">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="2" customFormat="1">
       <c r="A29" s="2" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="B29" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="2" customFormat="1">
       <c r="A30" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B30" s="2">
         <v>0</v>
@@ -2012,129 +2023,195 @@
     </row>
     <row r="31" spans="1:4" s="2" customFormat="1">
       <c r="A31" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>67</v>
+        <v>32</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="2" customFormat="1">
       <c r="A32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="2" customFormat="1">
+      <c r="A33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="2" customFormat="1">
+      <c r="A34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="2" customFormat="1">
+      <c r="A35" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="2" customFormat="1">
+      <c r="A36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="2" customFormat="1">
+      <c r="A37" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="2" customFormat="1">
+      <c r="A38" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B38" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" s="2" customFormat="1">
-      <c r="A33" s="2" t="s">
+      <c r="C38" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="2" customFormat="1">
+      <c r="A39" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B39" s="11" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" s="1" customFormat="1">
-      <c r="A34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="1" t="s">
+      <c r="C39" s="11"/>
+    </row>
+    <row r="40" spans="1:3" s="1" customFormat="1">
+      <c r="A40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="2" customFormat="1">
-      <c r="A35" s="2" t="s">
+    <row r="41" spans="1:3" s="2" customFormat="1">
+      <c r="A41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B41" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="2" customFormat="1">
-      <c r="A36" s="2" t="s">
+    <row r="42" spans="1:3" s="2" customFormat="1">
+      <c r="A42" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B42" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:2" s="2" customFormat="1">
-      <c r="A37" s="2" t="s">
+    <row r="43" spans="1:3" s="2" customFormat="1">
+      <c r="A43" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" s="2" customFormat="1">
-      <c r="A38" s="2" t="s">
+      <c r="B43" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="2" customFormat="1">
+      <c r="A44" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" s="2" customFormat="1">
-      <c r="A39" s="2" t="s">
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="2" customFormat="1">
+      <c r="A45" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" s="2" customFormat="1">
-      <c r="A40" s="2" t="s">
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="2" customFormat="1">
+      <c r="A46" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" s="2" customFormat="1">
-      <c r="A41" s="2" t="s">
+      <c r="B46" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="2" customFormat="1">
+      <c r="A47" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="2" customFormat="1">
+      <c r="A48" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="2" customFormat="1">
+      <c r="A49" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" s="2" customFormat="1">
-      <c r="A42" s="2" t="s">
+      <c r="B49" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="2" customFormat="1">
+      <c r="A50" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B50" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:2" s="2" customFormat="1">
-      <c r="A43" s="2" t="s">
+    <row r="51" spans="1:2" s="2" customFormat="1">
+      <c r="A51" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" s="2" customFormat="1">
-      <c r="A44" s="2" t="s">
+      <c r="B51" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" s="2" customFormat="1">
+      <c r="A52" s="11" t="s">
         <v>37</v>
       </c>
+      <c r="B52" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C19 A2:B3 A13:B14 A24:B25 A35:B36 C1:C8 B42:B44 C22:C41" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C10 A2:B3 A15:B16 A28:B29 A41:B42 C13:C23 B50:B52 C26:C49" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A9:A10 A20:A21 A42:A43 A31:B32 L1:L8 L11:L44 G31:G32 G42:G44" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A11:A12 A24:A25 A50:A51 A37:B38 G50:G52 L1:L10 G37:G38 L13:L52" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"int,string,float,object"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B9:B10 B20:B21 M1:M8 M11:M44 H31:H32 H42:H44" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B8 B18:B19 B29:B30 B40:B41 D11:G19 A4:B6 A15:B17 A26:B28 A37:B39 D1:G8 D22:G30 D33:G41" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B11:B12 B24:B25 H50:H52 M1:M10 H37:H38 M13:M52" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:G10 A4:B6 A17:B19 A30:B32 A43:B45 B33:B36 B20:B23 B7:B10 D13:G23 D26:G36 D39:G49 B46:B49" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>